<commit_message>
Implemented new way for evaluating study
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Wykres zdobywania punktow.xlsx
+++ b/src/main/resources/static/Wykres zdobywania punktow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbalt\Desktop\Repo\PlayWithMe\smo\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CFA4DF9-6BF5-4E4F-80EC-76C1B76D1BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED29A98D-6DE4-401F-A3E0-9FCEED1B1559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="-16200" windowWidth="19410" windowHeight="15585" xr2:uid="{204F9154-5232-44B1-B6AF-A95E0FA8E040}"/>
+    <workbookView xWindow="-2115" yWindow="-16200" windowWidth="14445" windowHeight="15585" xr2:uid="{204F9154-5232-44B1-B6AF-A95E0FA8E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1044,7 +1044,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2248,7 +2247,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2259,8 @@
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>1</v>
       </c>
       <c r="B17" s="1">
@@ -2435,7 +2435,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="4">
         <v>2</v>
       </c>
       <c r="B18" s="1">
@@ -2464,7 +2464,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="4">
         <v>3</v>
       </c>
       <c r="B19" s="1">
@@ -2493,7 +2493,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>4</v>
       </c>
       <c r="B20" s="1">
@@ -2522,7 +2522,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>5</v>
       </c>
       <c r="B21" s="1">
@@ -2551,7 +2551,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="4">
         <v>6</v>
       </c>
       <c r="B22" s="1">
@@ -2580,7 +2580,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="4">
         <v>7</v>
       </c>
       <c r="B23" s="1">
@@ -2609,7 +2609,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="4">
         <v>8</v>
       </c>
       <c r="B24" s="1">
@@ -2638,7 +2638,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="4">
         <v>9</v>
       </c>
       <c r="B25" s="1">
@@ -2667,7 +2667,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="4">
         <v>10</v>
       </c>
       <c r="B26" s="1">
@@ -2696,7 +2696,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="4">
         <v>11</v>
       </c>
       <c r="B27" s="1">
@@ -2725,7 +2725,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="4">
         <v>12</v>
       </c>
       <c r="B28" s="1">
@@ -2754,7 +2754,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="4">
         <v>13</v>
       </c>
       <c r="B29" s="1">
@@ -2783,7 +2783,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="4">
         <v>14</v>
       </c>
       <c r="B30" s="1">
@@ -2812,7 +2812,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="4">
         <v>15</v>
       </c>
       <c r="B31" s="1">
@@ -2841,7 +2841,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="4">
         <v>16</v>
       </c>
       <c r="B32" s="1">
@@ -2870,7 +2870,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="4">
         <v>17</v>
       </c>
       <c r="B33" s="1">
@@ -2899,7 +2899,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="4">
         <v>18</v>
       </c>
       <c r="B34" s="1">
@@ -2928,7 +2928,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="4">
         <v>19</v>
       </c>
       <c r="B35" s="1">
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="4">
         <v>20</v>
       </c>
       <c r="B36" s="1">

</xml_diff>

<commit_message>
Fix calculator choice logic and added tests
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Wykres zdobywania punktow.xlsx
+++ b/src/main/resources/static/Wykres zdobywania punktow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbalt\Desktop\Repo\PlayWithMe\smo\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED29A98D-6DE4-401F-A3E0-9FCEED1B1559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4023500-D69C-4DD4-B63F-2B332F5A8150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2115" yWindow="-16200" windowWidth="14445" windowHeight="15585" xr2:uid="{204F9154-5232-44B1-B6AF-A95E0FA8E040}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{204F9154-5232-44B1-B6AF-A95E0FA8E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$B$16</c:f>
+              <c:f>Arkusz1!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -249,7 +249,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$B$17:$B$36</c:f>
+              <c:f>Arkusz1!$B$10:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -328,7 +328,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$C$16</c:f>
+              <c:f>Arkusz1!$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -351,7 +351,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$C$17:$C$36</c:f>
+              <c:f>Arkusz1!$C$10:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -430,7 +430,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$D$16</c:f>
+              <c:f>Arkusz1!$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -453,7 +453,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$D$17:$D$36</c:f>
+              <c:f>Arkusz1!$D$10:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -532,7 +532,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$E$16</c:f>
+              <c:f>Arkusz1!$E$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -555,7 +555,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$E$17:$E$36</c:f>
+              <c:f>Arkusz1!$E$10:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -634,7 +634,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$F$16</c:f>
+              <c:f>Arkusz1!$F$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -657,7 +657,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$F$17:$F$36</c:f>
+              <c:f>Arkusz1!$F$10:$F$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -736,7 +736,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$G$16</c:f>
+              <c:f>Arkusz1!$G$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -761,7 +761,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$G$17:$G$36</c:f>
+              <c:f>Arkusz1!$G$10:$G$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -840,7 +840,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$H$16</c:f>
+              <c:f>Arkusz1!$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -865,7 +865,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$H$17:$H$36</c:f>
+              <c:f>Arkusz1!$H$10:$H$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -944,7 +944,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz1!$I$16</c:f>
+              <c:f>Arkusz1!$I$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -969,7 +969,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz1!$I$17:$I$36</c:f>
+              <c:f>Arkusz1!$I$10:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1065,7 +1065,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$A$16</c15:sqref>
+                          <c15:sqref>Arkusz1!$A$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1094,7 +1094,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Arkusz1!$A$17:$A$36</c15:sqref>
+                          <c15:sqref>Arkusz1!$A$10:$A$29</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1912,13 +1912,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>49695</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>11595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>712304</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>41413</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2244,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4197024C-E856-40D0-BF8B-A2134227E2DB}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,38 +2376,241 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1">
+        <v>69</v>
+      </c>
+      <c r="F10" s="1">
+        <v>100</v>
+      </c>
+      <c r="G10" s="1">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1">
+        <v>69</v>
+      </c>
+      <c r="F11" s="1">
+        <v>100</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1">
+        <v>69</v>
+      </c>
+      <c r="F12" s="1">
+        <v>100</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1">
+        <v>55</v>
+      </c>
+      <c r="I12" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1">
+        <v>69</v>
+      </c>
+      <c r="F13" s="1">
+        <v>100</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1">
+        <v>70</v>
+      </c>
+      <c r="I13" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1">
+        <v>69</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1">
+        <v>25</v>
+      </c>
+      <c r="H14" s="1">
+        <v>85</v>
+      </c>
+      <c r="I14" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1">
+        <v>69</v>
+      </c>
+      <c r="F15" s="1">
+        <v>100</v>
+      </c>
+      <c r="G15" s="1">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1">
+        <v>100</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100</v>
+      </c>
+    </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="A16" s="4">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
         <v>9</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>8</v>
+      <c r="C16" s="1">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1">
+        <v>69</v>
+      </c>
+      <c r="F16" s="1">
+        <v>100</v>
+      </c>
+      <c r="G16" s="1">
+        <v>35</v>
+      </c>
+      <c r="H16" s="1">
+        <v>100</v>
+      </c>
+      <c r="I16" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1">
         <v>9</v>
@@ -2425,18 +2628,18 @@
         <v>100</v>
       </c>
       <c r="G17" s="1">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="H17" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="I17" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1">
         <v>9</v>
@@ -2454,18 +2657,18 @@
         <v>100</v>
       </c>
       <c r="G18" s="1">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="H18" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="I18" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1">
         <v>9</v>
@@ -2483,18 +2686,18 @@
         <v>100</v>
       </c>
       <c r="G19" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H19" s="1">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="I19" s="1">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
         <v>9</v>
@@ -2512,18 +2715,18 @@
         <v>100</v>
       </c>
       <c r="G20" s="1">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="H20" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="I20" s="1">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1">
         <v>9</v>
@@ -2541,18 +2744,18 @@
         <v>100</v>
       </c>
       <c r="G21" s="1">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="H21" s="1">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="I21" s="1">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B22" s="1">
         <v>9</v>
@@ -2570,7 +2773,7 @@
         <v>100</v>
       </c>
       <c r="G22" s="1">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1">
         <v>100</v>
@@ -2581,7 +2784,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1">
         <v>9</v>
@@ -2599,7 +2802,7 @@
         <v>100</v>
       </c>
       <c r="G23" s="1">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="H23" s="1">
         <v>100</v>
@@ -2610,7 +2813,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1">
         <v>9</v>
@@ -2628,7 +2831,7 @@
         <v>100</v>
       </c>
       <c r="G24" s="1">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="H24" s="1">
         <v>100</v>
@@ -2639,7 +2842,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <v>9</v>
@@ -2657,7 +2860,7 @@
         <v>100</v>
       </c>
       <c r="G25" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="H25" s="1">
         <v>100</v>
@@ -2668,7 +2871,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B26" s="1">
         <v>9</v>
@@ -2686,7 +2889,7 @@
         <v>100</v>
       </c>
       <c r="G26" s="1">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="H26" s="1">
         <v>100</v>
@@ -2697,7 +2900,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1">
         <v>9</v>
@@ -2715,7 +2918,7 @@
         <v>100</v>
       </c>
       <c r="G27" s="1">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="H27" s="1">
         <v>100</v>
@@ -2726,7 +2929,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>9</v>
@@ -2744,7 +2947,7 @@
         <v>100</v>
       </c>
       <c r="G28" s="1">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="H28" s="1">
         <v>100</v>
@@ -2755,7 +2958,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1">
         <v>9</v>
@@ -2773,215 +2976,12 @@
         <v>100</v>
       </c>
       <c r="G29" s="1">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1">
         <v>100</v>
       </c>
       <c r="I29" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>14</v>
-      </c>
-      <c r="B30" s="1">
-        <v>9</v>
-      </c>
-      <c r="C30" s="1">
-        <v>24</v>
-      </c>
-      <c r="D30" s="1">
-        <v>44</v>
-      </c>
-      <c r="E30" s="1">
-        <v>69</v>
-      </c>
-      <c r="F30" s="1">
-        <v>100</v>
-      </c>
-      <c r="G30" s="1">
-        <v>70</v>
-      </c>
-      <c r="H30" s="1">
-        <v>100</v>
-      </c>
-      <c r="I30" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>15</v>
-      </c>
-      <c r="B31" s="1">
-        <v>9</v>
-      </c>
-      <c r="C31" s="1">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1">
-        <v>44</v>
-      </c>
-      <c r="E31" s="1">
-        <v>69</v>
-      </c>
-      <c r="F31" s="1">
-        <v>100</v>
-      </c>
-      <c r="G31" s="1">
-        <v>75</v>
-      </c>
-      <c r="H31" s="1">
-        <v>100</v>
-      </c>
-      <c r="I31" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1">
-        <v>9</v>
-      </c>
-      <c r="C32" s="1">
-        <v>24</v>
-      </c>
-      <c r="D32" s="1">
-        <v>44</v>
-      </c>
-      <c r="E32" s="1">
-        <v>69</v>
-      </c>
-      <c r="F32" s="1">
-        <v>100</v>
-      </c>
-      <c r="G32" s="1">
-        <v>80</v>
-      </c>
-      <c r="H32" s="1">
-        <v>100</v>
-      </c>
-      <c r="I32" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>17</v>
-      </c>
-      <c r="B33" s="1">
-        <v>9</v>
-      </c>
-      <c r="C33" s="1">
-        <v>24</v>
-      </c>
-      <c r="D33" s="1">
-        <v>44</v>
-      </c>
-      <c r="E33" s="1">
-        <v>69</v>
-      </c>
-      <c r="F33" s="1">
-        <v>100</v>
-      </c>
-      <c r="G33" s="1">
-        <v>85</v>
-      </c>
-      <c r="H33" s="1">
-        <v>100</v>
-      </c>
-      <c r="I33" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>18</v>
-      </c>
-      <c r="B34" s="1">
-        <v>9</v>
-      </c>
-      <c r="C34" s="1">
-        <v>24</v>
-      </c>
-      <c r="D34" s="1">
-        <v>44</v>
-      </c>
-      <c r="E34" s="1">
-        <v>69</v>
-      </c>
-      <c r="F34" s="1">
-        <v>100</v>
-      </c>
-      <c r="G34" s="1">
-        <v>90</v>
-      </c>
-      <c r="H34" s="1">
-        <v>100</v>
-      </c>
-      <c r="I34" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>19</v>
-      </c>
-      <c r="B35" s="1">
-        <v>9</v>
-      </c>
-      <c r="C35" s="1">
-        <v>24</v>
-      </c>
-      <c r="D35" s="1">
-        <v>44</v>
-      </c>
-      <c r="E35" s="1">
-        <v>69</v>
-      </c>
-      <c r="F35" s="1">
-        <v>100</v>
-      </c>
-      <c r="G35" s="1">
-        <v>95</v>
-      </c>
-      <c r="H35" s="1">
-        <v>100</v>
-      </c>
-      <c r="I35" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>20</v>
-      </c>
-      <c r="B36" s="1">
-        <v>9</v>
-      </c>
-      <c r="C36" s="1">
-        <v>24</v>
-      </c>
-      <c r="D36" s="1">
-        <v>44</v>
-      </c>
-      <c r="E36" s="1">
-        <v>69</v>
-      </c>
-      <c r="F36" s="1">
-        <v>100</v>
-      </c>
-      <c r="G36" s="1">
-        <v>100</v>
-      </c>
-      <c r="H36" s="1">
-        <v>100</v>
-      </c>
-      <c r="I36" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>